<commit_message>
Added a new oligo probe panel
Closes #83
</commit_message>
<xml_diff>
--- a/cosmx/latest/cosmx.xlsx
+++ b/cosmx/latest/cosmx.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="383">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -357,10 +357,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
   </si>
   <si>
-    <t>DBiT</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000222</t>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
   </si>
   <si>
     <t>SIMS</t>
@@ -459,6 +459,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
     <t>MERFISH</t>
   </si>
   <si>
@@ -513,6 +519,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
   </si>
   <si>
+    <t>MS Lipidomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
     <t>analyte_class</t>
   </si>
   <si>
@@ -624,40 +642,106 @@
     <t>acquisition_instrument_vendor</t>
   </si>
   <si>
+    <t>BGI Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024848</t>
+  </si>
+  <si>
+    <t>Cytiva</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023581</t>
+  </si>
+  <si>
+    <t>Thermo Fisher Scientific</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_008452</t>
+  </si>
+  <si>
+    <t>Zeiss Microscopy</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023607</t>
+  </si>
+  <si>
+    <t>GE Healthcare</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025461</t>
+  </si>
+  <si>
+    <t>Leica Microsystems</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_008960</t>
+  </si>
+  <si>
+    <t>Akoya Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023774</t>
+  </si>
+  <si>
+    <t>NanoString</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023912</t>
+  </si>
+  <si>
+    <t>Element Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026453</t>
+  </si>
+  <si>
+    <t>Andor</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023609</t>
+  </si>
+  <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
+    <t>Illumina</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_010233</t>
+  </si>
+  <si>
+    <t>Ionpath</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023605</t>
+  </si>
+  <si>
     <t>In-House</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
   </si>
   <si>
-    <t>BGI Genomics</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024848</t>
-  </si>
-  <si>
     <t>Resolve Biosciences</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023911</t>
   </si>
   <si>
-    <t>Cytiva</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023581</t>
-  </si>
-  <si>
-    <t>Thermo Fisher Scientific</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_008452</t>
-  </si>
-  <si>
-    <t>Zeiss Microscopy</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023607</t>
+    <t>Singular Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026683</t>
+  </si>
+  <si>
+    <t>Vizgen</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026274</t>
   </si>
   <si>
     <t>Standard BioTools (Fluidigm)</t>
@@ -666,12 +750,6 @@
     <t>https://identifiers.org/RRID:SCR_023606</t>
   </si>
   <si>
-    <t>GE Healthcare</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_025461</t>
-  </si>
-  <si>
     <t>Sciex</t>
   </si>
   <si>
@@ -684,18 +762,6 @@
     <t>https://identifiers.org/RRID:SCR_017365</t>
   </si>
   <si>
-    <t>Leica Microsystems</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_008960</t>
-  </si>
-  <si>
-    <t>Akoya Biosciences</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023774</t>
-  </si>
-  <si>
     <t>Evident Scientific (Olympus)</t>
   </si>
   <si>
@@ -720,48 +786,18 @@
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
-    <t>NanoString</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023912</t>
-  </si>
-  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_017105</t>
   </si>
   <si>
-    <t>Andor</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023609</t>
-  </si>
-  <si>
-    <t>Huron Digital Pathology</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024996</t>
-  </si>
-  <si>
-    <t>Illumina</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_010233</t>
-  </si>
-  <si>
     <t>Motic</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024856</t>
   </si>
   <si>
-    <t>Ionpath</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023605</t>
-  </si>
-  <si>
     <t>acquisition_instrument_model</t>
   </si>
   <si>
@@ -813,6 +849,12 @@
     <t>https://identifiers.org/RRID:SCR_021658</t>
   </si>
   <si>
+    <t>timsTOF Ultra 2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026541</t>
+  </si>
+  <si>
     <t>Lightsheet 7</t>
   </si>
   <si>
@@ -831,12 +873,30 @@
     <t>https://identifiers.org/RRID:SCR_024847</t>
   </si>
   <si>
+    <t>timsTOF Pro</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026544</t>
+  </si>
+  <si>
     <t>Unknown</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
   </si>
   <si>
+    <t>AVITI</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026452</t>
+  </si>
+  <si>
+    <t>timsTOF Pro 2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026545</t>
+  </si>
+  <si>
     <t>Q Exactive UHMR</t>
   </si>
   <si>
@@ -849,12 +909,24 @@
     <t>https://identifiers.org/RRID:SCR_020565</t>
   </si>
   <si>
+    <t>timsTOF SCP</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026542</t>
+  </si>
+  <si>
     <t>Zyla 4.2 sCMOS</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023610</t>
   </si>
   <si>
+    <t>Helios</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_019916</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -867,12 +939,30 @@
     <t>https://identifiers.org/RRID:SCR_020517</t>
   </si>
   <si>
+    <t>timsTOF Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026540</t>
+  </si>
+  <si>
     <t>BZ-X800</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023617</t>
   </si>
   <si>
+    <t>CyTOF 2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026551</t>
+  </si>
+  <si>
+    <t>G4X Spatial Sequencer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026684</t>
+  </si>
+  <si>
     <t>NextSeq 500</t>
   </si>
   <si>
@@ -897,6 +987,12 @@
     <t>https://identifiers.org/RRID:SCR_024568</t>
   </si>
   <si>
+    <t>CyTOF XT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026344</t>
+  </si>
+  <si>
     <t>NanoZoomer-SQ</t>
   </si>
   <si>
@@ -939,6 +1035,12 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>timsTOF HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026543</t>
+  </si>
+  <si>
     <t>PhenoImager Fusion</t>
   </si>
   <si>
@@ -1017,6 +1119,12 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>MERSCOPE</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000404</t>
+  </si>
+  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -1059,6 +1167,12 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
+    <t>MERSCOPE Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026273</t>
+  </si>
+  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1185,6 +1299,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Prime 5K Human Pan Tissue &amp; Pathways Panel; PN 1000724</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000426</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
   </si>
   <si>
@@ -1245,6 +1365,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Human Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-H-USCP-1KP-R</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000430</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
@@ -1287,7 +1413,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-01-08T12:49:57-08:00</t>
+    <t>2025-04-08T15:27:32-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1449,91 +1575,91 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>268</v>
+        <v>306</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>269</v>
+        <v>307</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>280</v>
+        <v>318</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>281</v>
+        <v>319</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>283</v>
+        <v>321</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>284</v>
+        <v>322</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>285</v>
+        <v>323</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>291</v>
+        <v>329</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>292</v>
+        <v>330</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>293</v>
+        <v>331</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>294</v>
+        <v>332</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>295</v>
+        <v>333</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>296</v>
+        <v>334</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>297</v>
+        <v>335</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>298</v>
+        <v>336</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>299</v>
+        <v>337</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>326</v>
+        <v>368</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>327</v>
+        <v>369</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>328</v>
+        <v>370</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>329</v>
+        <v>371</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>330</v>
+        <v>372</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>331</v>
+        <v>373</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>332</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2">
@@ -1541,13 +1667,13 @@
         <v>26</v>
       </c>
       <c r="AG2" t="s" s="34">
-        <v>333</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="22">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$38</formula1>
+      <formula1>'dataset_type'!$A$1:$A$41</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1556,10 +1682,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$23</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$66</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1612,7 +1738,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$13</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1638,10 +1764,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -1659,10 +1785,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -1680,18 +1806,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>279</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -1701,7 +1827,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1709,106 +1835,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>300</v>
+        <v>338</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>301</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>302</v>
+        <v>340</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>303</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>304</v>
+        <v>342</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>305</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>306</v>
+        <v>344</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>307</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>308</v>
+        <v>346</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>309</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>310</v>
+        <v>348</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>311</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>312</v>
+        <v>350</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>313</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>314</v>
+        <v>352</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>315</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>316</v>
+        <v>354</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>317</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>319</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>320</v>
+        <v>358</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>321</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>322</v>
+        <v>360</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>323</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>324</v>
+        <v>362</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>325</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>364</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>366</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -1826,12 +1968,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1855,16 +1997,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>376</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>377</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>337</v>
+        <v>379</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>339</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2">
@@ -1872,13 +2014,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>336</v>
+        <v>378</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>338</v>
+        <v>380</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>340</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +2030,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2196,6 +2338,30 @@
       </c>
       <c r="B38" t="s" s="0">
         <v>79</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2213,130 +2379,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2354,12 +2520,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2369,7 +2535,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2377,186 +2543,210 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>162</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>169</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2566,7 +2756,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2574,418 +2764,530 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>165</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>171</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>173</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>179</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>181</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>183</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>185</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>187</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>189</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>191</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>193</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>195</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>197</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>201</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>203</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>205</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>239</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>241</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>253</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>261</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>265</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>267</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>280</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>282</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3003,42 +3305,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>273</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>274</v>
+        <v>312</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>275</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>276</v>
+        <v>314</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>277</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>279</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3056,26 +3358,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>273</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>274</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>275</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>276</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>277</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -3093,18 +3395,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>287</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>288</v>
+        <v>326</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>289</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>